<commit_message>
Added ability to filter by calendar day for NSE calculation in daily sf streamflow script
</commit_message>
<xml_diff>
--- a/calibration/cal_parameter_values.xlsx
+++ b/calibration/cal_parameter_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaengott\Documents\Projects\Russian_River\RR_GSFLOW\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B793DAE9-A567-4314-9DFB-9913328FF323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FE061-8C67-40B7-BD11-B2651D8E6F7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8568" xr2:uid="{6750919F-702D-4986-8FE3-1BA04FF192B2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>ssr2gw_rate</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>Subbasin 13</t>
+  </si>
+  <si>
+    <t>Subbasin 22</t>
+  </si>
+  <si>
+    <t>NSE nov-apr</t>
+  </si>
+  <si>
+    <t>NSE all positve</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>apr</t>
   </si>
 </sst>
 </file>
@@ -146,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -156,12 +174,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,9 +187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -189,6 +198,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103F6FB5-3E2E-4EB0-9C14-4EB1E1BCF255}">
-  <dimension ref="A3:S17"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,46 +536,102 @@
     <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L1" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="O1" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="R1" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="U1" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5" t="s">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="4" t="s">
+      <c r="O3" s="16"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -566,13 +643,13 @@
       <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -584,13 +661,13 @@
       <c r="M4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -602,18 +679,27 @@
       <c r="S4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>0.34143299999999999</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>0.98977300000000001</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>1</v>
       </c>
       <c r="E5" s="2">
@@ -622,91 +708,95 @@
       <c r="F5" s="2">
         <v>0.99741500000000005</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>0.86703300000000005</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>0.99336000000000002</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="10"/>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>0.15</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>0.15</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <v>0.15</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>0.15</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>0.15</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="14">
         <v>0.15</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="13">
         <v>0.15</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>0.15</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="10">
         <v>0.15</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="10"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9">
+      <c r="B7" s="7"/>
+      <c r="E7" s="7">
         <v>0.70339499999999999</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>1.241687</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="10">
         <v>4.8350499999999998</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="13"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="13"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H7" s="13"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="10"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>0</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>33.589250999999997</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <v>64.8</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>7</v>
       </c>
       <c r="F8" s="2">
@@ -715,30 +805,31 @@
       <c r="G8" s="2">
         <v>58.088900000000002</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="13">
         <v>0</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <v>22.569901000000002</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="10">
         <v>50.133299999999998</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N8" s="7"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="10"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>0</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>1.5989999999999999E-3</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <v>1.223E-2</v>
       </c>
       <c r="E9" s="2">
@@ -750,100 +841,103 @@
       <c r="G9" s="2">
         <v>5.4559999999999999E-3</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="13">
         <v>0</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <v>1.3680000000000001E-3</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="10">
         <v>3.8639999999999998E-3</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="13"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N9" s="7"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="10"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>0.04</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>0.04</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="14">
         <v>0.04</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>0.04</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="11">
         <v>0.04</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="12">
         <v>0.04</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="13"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="10"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>1E-3</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>1E-3</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="11">
         <v>1E-3</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <v>1E-3</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="13"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="10"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <v>5.1525639999999999</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>9.7200000000000006</v>
       </c>
       <c r="E12" s="2">
@@ -852,68 +946,70 @@
       <c r="F12" s="2">
         <v>4.6163020000000001</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="14">
         <v>8.64</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>0</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="8">
         <v>4.4077479999999998</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="10">
         <v>10.74666</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="10"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>0</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>0.48712100000000003</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>0.66666999999999998</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>0.5</v>
       </c>
       <c r="F13" s="2">
         <v>0.79645500000000002</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="14">
         <v>1</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <v>0</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <v>0.63566199999999995</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="10">
         <v>1</v>
       </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="13"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="10"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>0</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <v>5.1000000000000004E-4</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>4.0850000000000001E-3</v>
       </c>
       <c r="E14" s="2">
@@ -925,39 +1021,78 @@
       <c r="G14" s="2">
         <v>2.673E-3</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>0</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>3.7800000000000003E-4</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="10">
         <v>1.17E-3</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="13"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="10"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="2">
+        <f>365-61</f>
+        <v>304</v>
+      </c>
+      <c r="G19" s="2">
+        <f>365-31</f>
+        <v>334</v>
+      </c>
+      <c r="H19" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="2">
+        <f>F19/365</f>
+        <v>0.83287671232876714</v>
+      </c>
+      <c r="G20" s="2">
+        <f>G19/365</f>
+        <v>0.91506849315068495</v>
+      </c>
+      <c r="H20" s="2">
+        <f>H19/365</f>
+        <v>0.24657534246575341</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A5:A14">
     <sortCondition ref="A5:A14"/>
   </sortState>
   <mergeCells count="6">
+    <mergeCell ref="Q3:S3"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added mean percent error and mean absolute percent error to daily sf cal script
</commit_message>
<xml_diff>
--- a/calibration/cal_parameter_values.xlsx
+++ b/calibration/cal_parameter_values.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaengott\Documents\Projects\Russian_River\RR_GSFLOW\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FE061-8C67-40B7-BD11-B2651D8E6F7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8881F93B-0439-4E66-9C68-3D44EACB388B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8568" xr2:uid="{6750919F-702D-4986-8FE3-1BA04FF192B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8568" activeTab="1" xr2:uid="{6750919F-702D-4986-8FE3-1BA04FF192B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>ssr2gw_rate</t>
   </si>
@@ -95,9 +96,6 @@
     <t>NSE nov-apr</t>
   </si>
   <si>
-    <t>NSE all positve</t>
-  </si>
-  <si>
     <t>nov</t>
   </si>
   <si>
@@ -105,6 +103,42 @@
   </si>
   <si>
     <t>apr</t>
+  </si>
+  <si>
+    <t>subbasin_1</t>
+  </si>
+  <si>
+    <t>subbasin_2</t>
+  </si>
+  <si>
+    <t>subbasin_3</t>
+  </si>
+  <si>
+    <t>subbasin_5</t>
+  </si>
+  <si>
+    <t>subbasin_6</t>
+  </si>
+  <si>
+    <t>subbasin_13</t>
+  </si>
+  <si>
+    <t>subbasin_22</t>
+  </si>
+  <si>
+    <t>MPE nov-apr</t>
+  </si>
+  <si>
+    <t>MAPE nov-apr</t>
+  </si>
+  <si>
+    <t>NSE all positive</t>
+  </si>
+  <si>
+    <t>MPE all positive</t>
+  </si>
+  <si>
+    <t>MAPE all positive</t>
   </si>
 </sst>
 </file>
@@ -164,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -198,6 +232,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,9 +244,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103F6FB5-3E2E-4EB0-9C14-4EB1E1BCF255}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A3:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,89 +575,37 @@
     <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="F1" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="I1" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L1" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="O1" s="2">
-        <v>0.61</v>
-      </c>
-      <c r="R1" s="2">
-        <v>0.68</v>
-      </c>
-      <c r="U1" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.74</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.63</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0.77</v>
-      </c>
-    </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="15" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="15" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18" t="s">
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
       <c r="T3" s="7"/>
       <c r="U3" s="2" t="s">
         <v>19</v>
@@ -1046,13 +1033,13 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -1097,4 +1084,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E07B6D-1D3C-4966-9EFD-6814E2737455}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="20">
+        <v>0.72</v>
+      </c>
+      <c r="C2" s="20">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D2" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0.67</v>
+      </c>
+      <c r="F2" s="20">
+        <v>0.61</v>
+      </c>
+      <c r="G2" s="20">
+        <v>0.68</v>
+      </c>
+      <c r="H2" s="20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0.74</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.08</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0.69</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0.63</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0.69</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="21">
+        <v>84.29</v>
+      </c>
+      <c r="C5" s="21">
+        <v>163.22999999999999</v>
+      </c>
+      <c r="D5" s="21">
+        <v>6.53</v>
+      </c>
+      <c r="E5" s="21">
+        <v>149</v>
+      </c>
+      <c r="F5" s="21">
+        <v>137.15</v>
+      </c>
+      <c r="G5" s="21">
+        <v>206.54</v>
+      </c>
+      <c r="H5" s="21">
+        <v>136.44999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="21">
+        <v>74.040000000000006</v>
+      </c>
+      <c r="C6" s="21">
+        <v>142.03</v>
+      </c>
+      <c r="D6" s="21">
+        <v>-46.66</v>
+      </c>
+      <c r="E6" s="21">
+        <v>133.66999999999999</v>
+      </c>
+      <c r="F6" s="21">
+        <v>101</v>
+      </c>
+      <c r="G6" s="21">
+        <v>171.77</v>
+      </c>
+      <c r="H6" s="21">
+        <v>80.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="21">
+        <v>112.89</v>
+      </c>
+      <c r="C8" s="21">
+        <v>197.92</v>
+      </c>
+      <c r="D8" s="21">
+        <v>115.58</v>
+      </c>
+      <c r="E8" s="21">
+        <v>182.71</v>
+      </c>
+      <c r="F8" s="21">
+        <v>162.66999999999999</v>
+      </c>
+      <c r="G8" s="21">
+        <v>226.91</v>
+      </c>
+      <c r="H8" s="21">
+        <v>161.88999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="21">
+        <v>104.13</v>
+      </c>
+      <c r="C9" s="21">
+        <v>181.71</v>
+      </c>
+      <c r="D9" s="21">
+        <v>104.12</v>
+      </c>
+      <c r="E9" s="21">
+        <v>173.39</v>
+      </c>
+      <c r="F9" s="21">
+        <v>141.13</v>
+      </c>
+      <c r="G9" s="21">
+        <v>203.16</v>
+      </c>
+      <c r="H9" s="21">
+        <v>134.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>